<commit_message>
Added chat bot (Not 100% working, but 80%'s done)
</commit_message>
<xml_diff>
--- a/public/MyPlannedCourses.xlsx
+++ b/public/MyPlannedCourses.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8FBAD7-7DC9-6A46-874A-E7BCE6D80FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497205F9-7F4E-1B4C-ACC8-CF0DCF5BDEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Class list" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="List_CourseID">Table_ClassList[Serial Number]</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Class list'!$B$6:$D$15,'Class list'!$I$6:$K$15,'Class list'!$M$6:$O$15</definedName>
     <definedName name="ScheduleEnd">#REF!</definedName>
     <definedName name="ScheduleSemester">#REF!</definedName>
     <definedName name="ScheduleStart">#REF!</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="9">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -57,12 +58,21 @@
   <si>
     <t>Course ID and Name</t>
   </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Total Credits</t>
+  </si>
+  <si>
+    <t>Note: Save the Plan as PDF or Print the page for each semester by simply pressing CTRL/COMMAND + P</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,13 +165,44 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <name val="Verdana"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1" tint="0.14999847407452621"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,8 +233,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -283,6 +330,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -295,7 +357,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -345,10 +407,16 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -360,6 +428,9 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Heading 1 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -370,47 +441,10 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Title 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="48">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Verdana"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Verdana"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -423,6 +457,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -441,6 +495,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -459,6 +533,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -475,7 +569,50 @@
       </font>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -488,6 +625,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -506,6 +663,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -524,6 +701,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -540,7 +737,50 @@
       </font>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -553,6 +793,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -571,6 +831,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -589,6 +869,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -605,18 +905,42 @@
       </font>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="16"/>
+        <color auto="1"/>
         <name val="Verdana"/>
         <family val="2"/>
         <scheme val="major"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -905,34 +1229,34 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleLight1 2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Custom 1" table="0" count="11" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="44"/>
-      <tableStyleElement type="headerRow" dxfId="43"/>
-      <tableStyleElement type="totalRow" dxfId="42"/>
-      <tableStyleElement type="firstRowStripe" dxfId="41"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="40"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="39"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="38"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="37"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="36"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="35"/>
-      <tableStyleElement type="pageFieldValues" dxfId="34"/>
+      <tableStyleElement type="wholeTable" dxfId="47"/>
+      <tableStyleElement type="headerRow" dxfId="46"/>
+      <tableStyleElement type="totalRow" dxfId="45"/>
+      <tableStyleElement type="firstRowStripe" dxfId="44"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="43"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="42"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="41"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="40"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="39"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="38"/>
+      <tableStyleElement type="pageFieldValues" dxfId="37"/>
     </tableStyle>
     <tableStyle name="PivotStyleLight1 2" table="0" count="8" xr9:uid="{DC5C22FD-AF7A-1D48-A057-A5DEB9115978}">
-      <tableStyleElement type="wholeTable" dxfId="33"/>
-      <tableStyleElement type="headerRow" dxfId="32"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="31"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="30"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="29"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="28"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="27"/>
-      <tableStyleElement type="pageFieldValues" dxfId="26"/>
+      <tableStyleElement type="wholeTable" dxfId="36"/>
+      <tableStyleElement type="headerRow" dxfId="35"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="34"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="33"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="32"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="31"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="30"/>
+      <tableStyleElement type="pageFieldValues" dxfId="29"/>
     </tableStyle>
     <tableStyle name="TableStyleLight1 2" pivot="0" count="5" xr9:uid="{D3C6B89F-4D0E-1849-8578-6A51D43AC2F4}">
-      <tableStyleElement type="wholeTable" dxfId="25"/>
-      <tableStyleElement type="headerRow" dxfId="24"/>
-      <tableStyleElement type="totalRow" dxfId="23"/>
-      <tableStyleElement type="firstColumn" dxfId="22"/>
-      <tableStyleElement type="lastColumn" dxfId="21"/>
+      <tableStyleElement type="wholeTable" dxfId="28"/>
+      <tableStyleElement type="headerRow" dxfId="27"/>
+      <tableStyleElement type="totalRow" dxfId="26"/>
+      <tableStyleElement type="firstColumn" dxfId="25"/>
+      <tableStyleElement type="lastColumn" dxfId="24"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2400,7 +2724,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="1644618" y="7144215"/>
-          <a:ext cx="748318" cy="680278"/>
+          <a:ext cx="832984" cy="680278"/>
           <a:chOff x="11310392" y="2730371"/>
           <a:chExt cx="749122" cy="695027"/>
         </a:xfrm>
@@ -3824,7 +4148,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="7684008">
-          <a:off x="2764356" y="7172283"/>
+          <a:off x="2849022" y="7172283"/>
           <a:ext cx="686943" cy="735955"/>
           <a:chOff x="11387833" y="3635337"/>
           <a:chExt cx="702284" cy="739582"/>
@@ -5256,7 +5580,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6589889" y="601818"/>
+          <a:off x="8494889" y="601818"/>
           <a:ext cx="0" cy="234043"/>
           <a:chOff x="15289984" y="599889"/>
           <a:chExt cx="1218209" cy="272143"/>
@@ -5492,16 +5816,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1262418</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>34751</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>366889</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2615820</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>14111</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>578555</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5516,8 +5840,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8825552" y="1717343"/>
-          <a:ext cx="2979761" cy="591403"/>
+          <a:off x="11464751" y="1707445"/>
+          <a:ext cx="4537249" cy="592666"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5559,13 +5883,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>432179</xdr:colOff>
+      <xdr:colOff>1735667</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>22747</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>329820</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -5582,8 +5906,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16297701" y="1740090"/>
-          <a:ext cx="3707641" cy="568656"/>
+          <a:off x="19797889" y="1744303"/>
+          <a:ext cx="4670778" cy="569919"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5626,18 +5950,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_ClassList" displayName="Table_ClassList" ref="B8:D15" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_ClassList" displayName="Table_ClassList" ref="B8:D15" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Serial Number" totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Course ID and Name" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Serial Number" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Course ID and Name" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BDD559BA-9D7C-4023-9F1F-B12393CCBF49}" name="Table_ClassList10" displayName="Table_ClassList10" ref="I8:K15" headerRowDxfId="1" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BDD559BA-9D7C-4023-9F1F-B12393CCBF49}" name="Table_ClassList10" displayName="Table_ClassList10" ref="I8:K15" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{636B3520-8BD9-4957-9D9C-4D2B87171C6B}" name="Serial Number" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
     <tableColumn id="2" xr3:uid="{40020D1C-889C-46E2-BA33-669742B8E1A7}" name="Course ID and Name" dataDxfId="10" totalsRowDxfId="9"/>
@@ -5648,11 +5972,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{0B95F143-7AC1-4632-B3DE-539EBC720588}" name="Table_ClassList11" displayName="Table_ClassList11" ref="M8:O15" headerRowDxfId="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{0B95F143-7AC1-4632-B3DE-539EBC720588}" name="Table_ClassList11" displayName="Table_ClassList11" ref="M8:O15" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BE7DEB95-093A-4D42-B18B-A09F737D2728}" name="Serial Number" totalsRowLabel="Total" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{E3C61B87-C0FB-4F08-8F3E-7C62DE4E751E}" name="Course ID and Name" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{AB9E1014-8B75-4B6D-A844-BC210042122D}" name="Credits" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{BE7DEB95-093A-4D42-B18B-A09F737D2728}" name="Serial Number" totalsRowLabel="Total" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{E3C61B87-C0FB-4F08-8F3E-7C62DE4E751E}" name="Course ID and Name" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{AB9E1014-8B75-4B6D-A844-BC210042122D}" name="Credits" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5867,26 +6191,26 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22" style="3" customWidth="1"/>
-    <col min="3" max="3" width="38.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="2.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
     <col min="8" max="8" width="0.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="39.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="59.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.1640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="24" style="1" customWidth="1"/>
-    <col min="14" max="14" width="37.1640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="61" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -5901,11 +6225,11 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:16" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="12" t="s">
         <v>0</v>
       </c>
@@ -5931,120 +6255,170 @@
     <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="20" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="20" t="s">
         <v>2</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N8" s="18" t="s">
+      <c r="N8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="O8" s="18" t="s">
+      <c r="O8" s="20" t="s">
         <v>2</v>
       </c>
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
     </row>
     <row r="10" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
     </row>
     <row r="11" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="M11" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
+      <c r="B12" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="M12" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
+      <c r="B13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
+      <c r="B14" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="17"/>
+      <c r="I15" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="I15" s="17" t="s">
+      <c r="J15" s="19"/>
+      <c r="K15" s="17"/>
+      <c r="M15" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="M15" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="N15" s="17"/>
+      <c r="N15" s="19"/>
       <c r="O15" s="17"/>
     </row>
     <row r="16" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6057,7 +6431,11 @@
       <c r="D20" s="8"/>
     </row>
     <row r="21" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
@@ -6099,15 +6477,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6419,6 +6788,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03380CC4-5E45-4F9B-AB2E-6D2C69B2C711}">
   <ds:schemaRefs>
@@ -6432,14 +6810,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EBB0510-F433-4EEE-B839-6F7BB0E54948}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35AE4578-397D-472A-82B2-5A96CF8D33B3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6460,6 +6830,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EBB0510-F433-4EEE-B839-6F7BB0E54948}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
fixed xlms files with logo and some UI fixes
</commit_message>
<xml_diff>
--- a/public/MyPlannedCourses.xlsx
+++ b/public/MyPlannedCourses.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497205F9-7F4E-1B4C-ACC8-CF0DCF5BDEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A740E8DB-F171-7949-8E0B-FFF3A4864CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="List_CourseID">Table_ClassList[Serial Number]</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Class list'!$B$6:$D$15,'Class list'!$I$6:$K$15,'Class list'!$M$6:$O$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Class list'!$B$7:$D$16,'Class list'!$I$7:$K$16,'Class list'!$M$7:$O$16</definedName>
     <definedName name="ScheduleEnd">#REF!</definedName>
     <definedName name="ScheduleSemester">#REF!</definedName>
     <definedName name="ScheduleStart">#REF!</definedName>
@@ -419,6 +419,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="3"/>
     </xf>
@@ -427,9 +430,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1276,13 +1276,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>267838</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>300571</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>994034</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>78145</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1298,7 +1298,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="1345582">
-          <a:off x="564171" y="7130349"/>
+          <a:off x="564171" y="7581904"/>
           <a:ext cx="726196" cy="680685"/>
           <a:chOff x="11243096" y="3646378"/>
           <a:chExt cx="726195" cy="691841"/>
@@ -2701,13 +2701,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1348285</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>314437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>417380</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>91604</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2723,7 +2723,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1644618" y="7144215"/>
+          <a:off x="1644618" y="7595770"/>
           <a:ext cx="832984" cy="680278"/>
           <a:chOff x="11310392" y="2730371"/>
           <a:chExt cx="749122" cy="695027"/>
@@ -4126,13 +4126,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>764294</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>367011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1500249</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>150843</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -4148,7 +4148,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="7684008">
-          <a:off x="2849022" y="7172283"/>
+          <a:off x="2849022" y="7623838"/>
           <a:ext cx="686943" cy="735955"/>
           <a:chOff x="11387833" y="3635337"/>
           <a:chExt cx="702284" cy="739582"/>
@@ -5752,13 +5752,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>11374</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5818,13 +5818,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>34751</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>366889</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>14111</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>578555</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5884,13 +5884,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>1735667</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>22747</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5946,11 +5946,55 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1142999</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3852332</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>395110</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B98EBAD-2CD2-EBF0-D369-3D553FFCF099}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12572999" y="0"/>
+          <a:ext cx="2709333" cy="2709332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_ClassList" displayName="Table_ClassList" ref="B8:D15" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_ClassList" displayName="Table_ClassList" ref="B9:D16" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Serial Number" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="19"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Course ID and Name" dataDxfId="18" totalsRowDxfId="17"/>
@@ -5961,7 +6005,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BDD559BA-9D7C-4023-9F1F-B12393CCBF49}" name="Table_ClassList10" displayName="Table_ClassList10" ref="I8:K15" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BDD559BA-9D7C-4023-9F1F-B12393CCBF49}" name="Table_ClassList10" displayName="Table_ClassList10" ref="I9:K16" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{636B3520-8BD9-4957-9D9C-4D2B87171C6B}" name="Serial Number" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
     <tableColumn id="2" xr3:uid="{40020D1C-889C-46E2-BA33-669742B8E1A7}" name="Course ID and Name" dataDxfId="10" totalsRowDxfId="9"/>
@@ -5972,7 +6016,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{0B95F143-7AC1-4632-B3DE-539EBC720588}" name="Table_ClassList11" displayName="Table_ClassList11" ref="M8:O15" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{0B95F143-7AC1-4632-B3DE-539EBC720588}" name="Table_ClassList11" displayName="Table_ClassList11" ref="M9:O16" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BE7DEB95-093A-4D42-B18B-A09F737D2728}" name="Serial Number" totalsRowLabel="Total" dataDxfId="4" totalsRowDxfId="3"/>
     <tableColumn id="2" xr3:uid="{E3C61B87-C0FB-4F08-8F3E-7C62DE4E751E}" name="Course ID and Name" dataDxfId="2" totalsRowDxfId="1"/>
@@ -6188,10 +6232,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6225,11 +6269,11 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:16" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="12" t="s">
         <v>0</v>
       </c>
@@ -6252,52 +6296,58 @@
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
     <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
-      <c r="B8" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="I8" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="O8" s="20" t="s">
-        <v>2</v>
-      </c>
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
+      <c r="B9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="I9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="19"/>
@@ -6317,24 +6367,14 @@
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
-      <c r="M11" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="O11" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
     </row>
     <row r="12" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="B12" s="19"/>
       <c r="C12" s="19"/>
-      <c r="D12" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="D12" s="19"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
@@ -6352,25 +6392,19 @@
       <c r="B13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="C13" s="19"/>
       <c r="D13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="J13" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
       <c r="M13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="19"/>
+      <c r="N13" s="19" t="s">
+        <v>6</v>
+      </c>
       <c r="O13" s="19" t="s">
         <v>6</v>
       </c>
@@ -6397,42 +6431,69 @@
       <c r="M14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="N14" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="N14" s="19"/>
       <c r="O14" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="O15" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="17"/>
-      <c r="I15" s="18" t="s">
+      <c r="C16" s="19"/>
+      <c r="D16" s="17"/>
+      <c r="I16" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="17"/>
-      <c r="M15" s="18" t="s">
+      <c r="J16" s="19"/>
+      <c r="K16" s="17"/>
+      <c r="M16" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="N15" s="19"/>
-      <c r="O15" s="17"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="17"/>
     </row>
-    <row r="16" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="17" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" spans="2:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+    <row r="20" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="2:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
     </row>
-    <row r="21" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="24" t="s">
+    <row r="22" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="23" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="21" t="s">
         <v>8</v>
       </c>
     </row>
@@ -6457,26 +6518,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6788,6 +6829,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6798,18 +6859,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03380CC4-5E45-4F9B-AB2E-6D2C69B2C711}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35AE4578-397D-472A-82B2-5A96CF8D33B3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6830,6 +6879,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03380CC4-5E45-4F9B-AB2E-6D2C69B2C711}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EBB0510-F433-4EEE-B839-6F7BB0E54948}">
   <ds:schemaRefs>

</xml_diff>